<commit_message>
Removed duplicate columns from linked tables
</commit_message>
<xml_diff>
--- a/sample_sales_mix.xlsx
+++ b/sample_sales_mix.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Anand\Auto Generate PPT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Anand\GitHub\excel-to-ppt-explainer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{394F6D00-18C5-4D30-BD24-17B7C598C429}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{533AA67F-6709-40F7-878F-AE6B0BD2B3B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -55,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="23">
   <si>
     <t>Category</t>
   </si>
@@ -115,6 +116,15 @@
   </si>
   <si>
     <t>Revenue (USD)</t>
+  </si>
+  <si>
+    <t>Perm Employee</t>
+  </si>
+  <si>
+    <t>Contract Employee</t>
+  </si>
+  <si>
+    <t>Total Employee</t>
   </si>
 </sst>
 </file>
@@ -186,6 +196,20 @@
   </cellStyles>
   <dxfs count="3">
     <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -214,20 +238,6 @@
         <bottom/>
       </border>
     </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-      </border>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -242,7 +252,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4B48E3AD-7671-4614-87CF-1E8B4C0FC318}" name="Raw_Data" displayName="Raw_Data" ref="A1:I7" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="1" tableBorderDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4B48E3AD-7671-4614-87CF-1E8B4C0FC318}" name="Raw_Data" displayName="Raw_Data" ref="A1:I7" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="1" tableBorderDxfId="0">
   <autoFilter ref="A1:I7" xr:uid="{4B48E3AD-7671-4614-87CF-1E8B4C0FC318}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{7F5D78E5-4BBD-48FD-B83B-25EB70AA534C}" name="Category"/>
@@ -254,6 +264,18 @@
     <tableColumn id="7" xr3:uid="{76AE53FF-F556-4285-9062-C783B6827E3E}" name="Retail%"/>
     <tableColumn id="8" xr3:uid="{C7C6B015-C22B-4B35-92B1-F1A0B4E07F8D}" name="Wholesale%"/>
     <tableColumn id="9" xr3:uid="{1F2638B4-ADA6-43B8-AA71-449AB09D4CDB}" name="Direct%"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{96C92FC0-CC00-43A8-A75C-6A98AC317203}" name="Table2" displayName="Table2" ref="A1:C5" totalsRowShown="0">
+  <autoFilter ref="A1:C5" xr:uid="{96C92FC0-CC00-43A8-A75C-6A98AC317203}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{0A4A384A-043C-486E-8D1E-C8F647463629}" name="Category"/>
+    <tableColumn id="2" xr3:uid="{F505B5F8-4515-4495-9F58-A95BD8451FCB}" name="Perm Employee"/>
+    <tableColumn id="3" xr3:uid="{480F3350-E73B-4FE0-8EEC-19134CC34B11}" name="Contract Employee"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -549,7 +571,7 @@
   <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -563,6 +585,9 @@
     <col min="7" max="7" width="9.44140625" customWidth="1"/>
     <col min="8" max="8" width="13.77734375" customWidth="1"/>
     <col min="9" max="9" width="9.5546875" customWidth="1"/>
+    <col min="12" max="12" width="10.44140625" customWidth="1"/>
+    <col min="13" max="13" width="16.109375" customWidth="1"/>
+    <col min="14" max="14" width="18.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
@@ -787,6 +812,9 @@
       <c r="F11" t="s">
         <v>8</v>
       </c>
+      <c r="G11" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="str" cm="1">
@@ -813,6 +841,10 @@
         <f t="array" ref="F12">SUM(_xlfn._xlws.FILTER(Raw_Data[Units Sold]*Raw_Data[Direct%],Raw_Data[Category]=A12))/SUM(_xlfn._xlws.FILTER(Raw_Data[Units Sold],Raw_Data[Category]=A12))</f>
         <v>9.545454545454545</v>
       </c>
+      <c r="G12" cm="1">
+        <f t="array" ref="G12">SUM(_xlfn._xlws.FILTER(Table2[Perm Employee],Table2[Category]=A12))+SUM(_xlfn._xlws.FILTER(Table2[Contract Employee],Table2[Category]=A12))</f>
+        <v>8</v>
+      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="str">
@@ -838,6 +870,10 @@
         <f t="array" ref="F13">SUM(_xlfn._xlws.FILTER(Raw_Data[Units Sold]*Raw_Data[Direct%],Raw_Data[Category]=A13))/SUM(_xlfn._xlws.FILTER(Raw_Data[Units Sold],Raw_Data[Category]=A13))</f>
         <v>13.125</v>
       </c>
+      <c r="G13" cm="1">
+        <f t="array" ref="G13">SUM(_xlfn._xlws.FILTER(Table2[Perm Employee],Table2[Category]=A13))+SUM(_xlfn._xlws.FILTER(Table2[Contract Employee],Table2[Category]=A13))</f>
+        <v>5</v>
+      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="str">
@@ -863,6 +899,10 @@
         <f t="array" ref="F14">SUM(_xlfn._xlws.FILTER(Raw_Data[Units Sold]*Raw_Data[Direct%],Raw_Data[Category]=A14))/SUM(_xlfn._xlws.FILTER(Raw_Data[Units Sold],Raw_Data[Category]=A14))</f>
         <v>0</v>
       </c>
+      <c r="G14" cm="1">
+        <f t="array" ref="G14">SUM(_xlfn._xlws.FILTER(Table2[Perm Employee],Table2[Category]=A14))+SUM(_xlfn._xlws.FILTER(Table2[Contract Employee],Table2[Category]=A14))</f>
+        <v>4</v>
+      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="str">
@@ -887,6 +927,83 @@
       <c r="F15" s="2" cm="1">
         <f t="array" ref="F15">SUM(_xlfn._xlws.FILTER(Raw_Data[Units Sold]*Raw_Data[Direct%],Raw_Data[Category]=A15))/SUM(_xlfn._xlws.FILTER(Raw_Data[Units Sold],Raw_Data[Category]=A15))</f>
         <v>0</v>
+      </c>
+      <c r="G15" cm="1">
+        <f t="array" ref="G15">SUM(_xlfn._xlws.FILTER(Table2[Perm Employee],Table2[Category]=A15))+SUM(_xlfn._xlws.FILTER(Table2[Contract Employee],Table2[Category]=A15))</f>
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F86C92D4-C475-4933-8F8E-E8E5C832E610}">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Allow summary columns to reference different tables (#11)
* Load tables from all sheets and clarify summary sheet flag

* Removed duplicate columns from linked tables
</commit_message>
<xml_diff>
--- a/sample_sales_mix.xlsx
+++ b/sample_sales_mix.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Anand\Auto Generate PPT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Anand\GitHub\excel-to-ppt-explainer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{394F6D00-18C5-4D30-BD24-17B7C598C429}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{533AA67F-6709-40F7-878F-AE6B0BD2B3B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -55,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="23">
   <si>
     <t>Category</t>
   </si>
@@ -115,6 +116,15 @@
   </si>
   <si>
     <t>Revenue (USD)</t>
+  </si>
+  <si>
+    <t>Perm Employee</t>
+  </si>
+  <si>
+    <t>Contract Employee</t>
+  </si>
+  <si>
+    <t>Total Employee</t>
   </si>
 </sst>
 </file>
@@ -186,6 +196,20 @@
   </cellStyles>
   <dxfs count="3">
     <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -214,20 +238,6 @@
         <bottom/>
       </border>
     </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-      </border>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -242,7 +252,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4B48E3AD-7671-4614-87CF-1E8B4C0FC318}" name="Raw_Data" displayName="Raw_Data" ref="A1:I7" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="1" tableBorderDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4B48E3AD-7671-4614-87CF-1E8B4C0FC318}" name="Raw_Data" displayName="Raw_Data" ref="A1:I7" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="1" tableBorderDxfId="0">
   <autoFilter ref="A1:I7" xr:uid="{4B48E3AD-7671-4614-87CF-1E8B4C0FC318}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{7F5D78E5-4BBD-48FD-B83B-25EB70AA534C}" name="Category"/>
@@ -254,6 +264,18 @@
     <tableColumn id="7" xr3:uid="{76AE53FF-F556-4285-9062-C783B6827E3E}" name="Retail%"/>
     <tableColumn id="8" xr3:uid="{C7C6B015-C22B-4B35-92B1-F1A0B4E07F8D}" name="Wholesale%"/>
     <tableColumn id="9" xr3:uid="{1F2638B4-ADA6-43B8-AA71-449AB09D4CDB}" name="Direct%"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{96C92FC0-CC00-43A8-A75C-6A98AC317203}" name="Table2" displayName="Table2" ref="A1:C5" totalsRowShown="0">
+  <autoFilter ref="A1:C5" xr:uid="{96C92FC0-CC00-43A8-A75C-6A98AC317203}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{0A4A384A-043C-486E-8D1E-C8F647463629}" name="Category"/>
+    <tableColumn id="2" xr3:uid="{F505B5F8-4515-4495-9F58-A95BD8451FCB}" name="Perm Employee"/>
+    <tableColumn id="3" xr3:uid="{480F3350-E73B-4FE0-8EEC-19134CC34B11}" name="Contract Employee"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -549,7 +571,7 @@
   <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -563,6 +585,9 @@
     <col min="7" max="7" width="9.44140625" customWidth="1"/>
     <col min="8" max="8" width="13.77734375" customWidth="1"/>
     <col min="9" max="9" width="9.5546875" customWidth="1"/>
+    <col min="12" max="12" width="10.44140625" customWidth="1"/>
+    <col min="13" max="13" width="16.109375" customWidth="1"/>
+    <col min="14" max="14" width="18.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
@@ -787,6 +812,9 @@
       <c r="F11" t="s">
         <v>8</v>
       </c>
+      <c r="G11" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="str" cm="1">
@@ -813,6 +841,10 @@
         <f t="array" ref="F12">SUM(_xlfn._xlws.FILTER(Raw_Data[Units Sold]*Raw_Data[Direct%],Raw_Data[Category]=A12))/SUM(_xlfn._xlws.FILTER(Raw_Data[Units Sold],Raw_Data[Category]=A12))</f>
         <v>9.545454545454545</v>
       </c>
+      <c r="G12" cm="1">
+        <f t="array" ref="G12">SUM(_xlfn._xlws.FILTER(Table2[Perm Employee],Table2[Category]=A12))+SUM(_xlfn._xlws.FILTER(Table2[Contract Employee],Table2[Category]=A12))</f>
+        <v>8</v>
+      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="str">
@@ -838,6 +870,10 @@
         <f t="array" ref="F13">SUM(_xlfn._xlws.FILTER(Raw_Data[Units Sold]*Raw_Data[Direct%],Raw_Data[Category]=A13))/SUM(_xlfn._xlws.FILTER(Raw_Data[Units Sold],Raw_Data[Category]=A13))</f>
         <v>13.125</v>
       </c>
+      <c r="G13" cm="1">
+        <f t="array" ref="G13">SUM(_xlfn._xlws.FILTER(Table2[Perm Employee],Table2[Category]=A13))+SUM(_xlfn._xlws.FILTER(Table2[Contract Employee],Table2[Category]=A13))</f>
+        <v>5</v>
+      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="str">
@@ -863,6 +899,10 @@
         <f t="array" ref="F14">SUM(_xlfn._xlws.FILTER(Raw_Data[Units Sold]*Raw_Data[Direct%],Raw_Data[Category]=A14))/SUM(_xlfn._xlws.FILTER(Raw_Data[Units Sold],Raw_Data[Category]=A14))</f>
         <v>0</v>
       </c>
+      <c r="G14" cm="1">
+        <f t="array" ref="G14">SUM(_xlfn._xlws.FILTER(Table2[Perm Employee],Table2[Category]=A14))+SUM(_xlfn._xlws.FILTER(Table2[Contract Employee],Table2[Category]=A14))</f>
+        <v>4</v>
+      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="str">
@@ -887,6 +927,83 @@
       <c r="F15" s="2" cm="1">
         <f t="array" ref="F15">SUM(_xlfn._xlws.FILTER(Raw_Data[Units Sold]*Raw_Data[Direct%],Raw_Data[Category]=A15))/SUM(_xlfn._xlws.FILTER(Raw_Data[Units Sold],Raw_Data[Category]=A15))</f>
         <v>0</v>
+      </c>
+      <c r="G15" cm="1">
+        <f t="array" ref="G15">SUM(_xlfn._xlws.FILTER(Table2[Perm Employee],Table2[Category]=A15))+SUM(_xlfn._xlws.FILTER(Table2[Contract Employee],Table2[Category]=A15))</f>
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F86C92D4-C475-4933-8F8E-E8E5C832E610}">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
In Sheet we have a table named Table1. In that table a new column is inserted with name 'Ratio (Contract to Perm)'. That columns value is computed by dividing two columns of same table. Formula used is '=[@[Contract Employee]]/[@[Perm Employee]]'
</commit_message>
<xml_diff>
--- a/sample_sales_mix.xlsx
+++ b/sample_sales_mix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Anand\GitHub\excel-to-ppt-explainer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{533AA67F-6709-40F7-878F-AE6B0BD2B3B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40D5B078-543C-495C-AA56-61149AF0BA6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="25">
   <si>
     <t>Category</t>
   </si>
@@ -125,6 +125,12 @@
   </si>
   <si>
     <t>Total Employee</t>
+  </si>
+  <si>
+    <t>Ratio (Contract to Perm)</t>
+  </si>
+  <si>
+    <t>Ratio (Perm to Contract)</t>
   </si>
 </sst>
 </file>
@@ -194,7 +200,10 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="4">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <border outline="0">
         <top style="thin">
@@ -252,7 +261,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4B48E3AD-7671-4614-87CF-1E8B4C0FC318}" name="Raw_Data" displayName="Raw_Data" ref="A1:I7" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="1" tableBorderDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4B48E3AD-7671-4614-87CF-1E8B4C0FC318}" name="Raw_Data" displayName="Raw_Data" ref="A1:I7" totalsRowShown="0" headerRowDxfId="3" headerRowBorderDxfId="2" tableBorderDxfId="1">
   <autoFilter ref="A1:I7" xr:uid="{4B48E3AD-7671-4614-87CF-1E8B4C0FC318}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{7F5D78E5-4BBD-48FD-B83B-25EB70AA534C}" name="Category"/>
@@ -270,12 +279,15 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{96C92FC0-CC00-43A8-A75C-6A98AC317203}" name="Table2" displayName="Table2" ref="A1:C5" totalsRowShown="0">
-  <autoFilter ref="A1:C5" xr:uid="{96C92FC0-CC00-43A8-A75C-6A98AC317203}"/>
-  <tableColumns count="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{96C92FC0-CC00-43A8-A75C-6A98AC317203}" name="Table2" displayName="Table2" ref="A1:D5" totalsRowShown="0">
+  <autoFilter ref="A1:D5" xr:uid="{96C92FC0-CC00-43A8-A75C-6A98AC317203}"/>
+  <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{0A4A384A-043C-486E-8D1E-C8F647463629}" name="Category"/>
     <tableColumn id="2" xr3:uid="{F505B5F8-4515-4495-9F58-A95BD8451FCB}" name="Perm Employee"/>
     <tableColumn id="3" xr3:uid="{480F3350-E73B-4FE0-8EEC-19134CC34B11}" name="Contract Employee"/>
+    <tableColumn id="4" xr3:uid="{BC93B0AB-3D51-4030-A2CF-D1E492059A91}" name="Ratio (Contract to Perm)" dataDxfId="0">
+      <calculatedColumnFormula>Table2[[#This Row],[Contract Employee]]/Table2[[#This Row],[Perm Employee]]</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -571,7 +583,7 @@
   <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -815,6 +827,9 @@
       <c r="G11" t="s">
         <v>22</v>
       </c>
+      <c r="H11" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="str" cm="1">
@@ -845,6 +860,10 @@
         <f t="array" ref="G12">SUM(_xlfn._xlws.FILTER(Table2[Perm Employee],Table2[Category]=A12))+SUM(_xlfn._xlws.FILTER(Table2[Contract Employee],Table2[Category]=A12))</f>
         <v>8</v>
       </c>
+      <c r="H12" cm="1">
+        <f t="array" ref="H12">SUM(_xlfn._xlws.FILTER(Table2[Ratio (Contract to Perm)],Table2[Category]=A12))</f>
+        <v>3</v>
+      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="str">
@@ -874,6 +893,10 @@
         <f t="array" ref="G13">SUM(_xlfn._xlws.FILTER(Table2[Perm Employee],Table2[Category]=A13))+SUM(_xlfn._xlws.FILTER(Table2[Contract Employee],Table2[Category]=A13))</f>
         <v>5</v>
       </c>
+      <c r="H13" cm="1">
+        <f t="array" ref="H13">SUM(_xlfn._xlws.FILTER(Table2[Ratio (Contract to Perm)],Table2[Category]=A13))</f>
+        <v>4</v>
+      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="str">
@@ -903,6 +926,10 @@
         <f t="array" ref="G14">SUM(_xlfn._xlws.FILTER(Table2[Perm Employee],Table2[Category]=A14))+SUM(_xlfn._xlws.FILTER(Table2[Contract Employee],Table2[Category]=A14))</f>
         <v>4</v>
       </c>
+      <c r="H14" cm="1">
+        <f t="array" ref="H14">SUM(_xlfn._xlws.FILTER(Table2[Ratio (Contract to Perm)],Table2[Category]=A14))</f>
+        <v>3</v>
+      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="str">
@@ -931,6 +958,10 @@
       <c r="G15" cm="1">
         <f t="array" ref="G15">SUM(_xlfn._xlws.FILTER(Table2[Perm Employee],Table2[Category]=A15))+SUM(_xlfn._xlws.FILTER(Table2[Contract Employee],Table2[Category]=A15))</f>
         <v>3</v>
+      </c>
+      <c r="H15" cm="1">
+        <f t="array" ref="H15">SUM(_xlfn._xlws.FILTER(Table2[Ratio (Contract to Perm)],Table2[Category]=A15))</f>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -943,15 +974,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F86C92D4-C475-4933-8F8E-E8E5C832E610}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C5"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="23.88671875" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -961,8 +996,11 @@
       <c r="C1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -972,8 +1010,12 @@
       <c r="C2">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D2">
+        <f>Table2[[#This Row],[Contract Employee]]/Table2[[#This Row],[Perm Employee]]</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -983,8 +1025,12 @@
       <c r="C3">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D3">
+        <f>Table2[[#This Row],[Contract Employee]]/Table2[[#This Row],[Perm Employee]]</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -994,8 +1040,12 @@
       <c r="C4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D4">
+        <f>Table2[[#This Row],[Contract Employee]]/Table2[[#This Row],[Perm Employee]]</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -1003,6 +1053,10 @@
         <v>1</v>
       </c>
       <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <f>Table2[[#This Row],[Contract Employee]]/Table2[[#This Row],[Perm Employee]]</f>
         <v>2</v>
       </c>
     </row>

</xml_diff>